<commit_message>
added support for led
</commit_message>
<xml_diff>
--- a/indieDT/PCB_pin_mapping.xlsx
+++ b/indieDT/PCB_pin_mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="427">
   <si>
     <t xml:space="preserve">Atmega 2560 16AU</t>
   </si>
@@ -1300,6 +1300,9 @@
   </si>
   <si>
     <t xml:space="preserve">AVCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X pin -37</t>
   </si>
 </sst>
 </file>
@@ -1456,7 +1459,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1533,18 +1536,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1567,14 +1558,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1687,29 +1670,29 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N103"/>
+  <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2354,29 +2337,29 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19" t="n">
+      <c r="A20" s="11" t="n">
         <v>17</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="20" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I20" s="19" t="n">
+      <c r="I20" s="11" t="n">
         <v>17</v>
       </c>
       <c r="J20" s="7" t="n">
@@ -2394,29 +2377,29 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="n">
+      <c r="A21" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="20" t="s">
+      <c r="E21" s="11"/>
+      <c r="F21" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I21" s="19" t="n">
+      <c r="I21" s="11" t="n">
         <v>18</v>
       </c>
       <c r="J21" s="7" t="n">
@@ -2445,7 +2428,7 @@
       <c r="G22" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="19" t="s">
         <v>93</v>
       </c>
       <c r="I22" s="11" t="n">
@@ -2475,7 +2458,7 @@
       <c r="G23" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H23" s="19" t="s">
         <v>97</v>
       </c>
       <c r="I23" s="11" t="n">
@@ -2513,7 +2496,7 @@
       <c r="G24" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="19" t="s">
         <v>102</v>
       </c>
       <c r="I24" s="11" t="n">
@@ -2551,7 +2534,7 @@
       <c r="G25" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="19" t="s">
         <v>107</v>
       </c>
       <c r="I25" s="11" t="n">
@@ -2570,29 +2553,29 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="n">
+      <c r="A26" s="11" t="n">
         <v>23</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20" t="s">
+      <c r="E26" s="11"/>
+      <c r="F26" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="22" t="s">
+      <c r="H26" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="I26" s="19" t="n">
+      <c r="I26" s="11" t="n">
         <v>23</v>
       </c>
       <c r="J26" s="7"/>
@@ -2625,13 +2608,13 @@
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
-      <c r="H27" s="23" t="s">
+      <c r="H27" s="20" t="s">
         <v>119</v>
       </c>
       <c r="I27" s="11" t="n">
         <v>24</v>
       </c>
-      <c r="J27" s="24"/>
+      <c r="J27" s="21"/>
       <c r="K27" s="8"/>
       <c r="L27" s="13" t="n">
         <v>56</v>
@@ -2659,7 +2642,7 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
-      <c r="H28" s="25" t="s">
+      <c r="H28" s="22" t="s">
         <v>124</v>
       </c>
       <c r="I28" s="11" t="n">
@@ -2693,13 +2676,13 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
-      <c r="H29" s="25" t="s">
+      <c r="H29" s="22" t="s">
         <v>129</v>
       </c>
       <c r="I29" s="11" t="n">
         <v>26</v>
       </c>
-      <c r="J29" s="24"/>
+      <c r="J29" s="21"/>
       <c r="K29" s="8"/>
       <c r="L29" s="13" t="n">
         <v>26</v>
@@ -2985,7 +2968,7 @@
       <c r="G38" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="H38" s="26" t="s">
+      <c r="H38" s="23" t="s">
         <v>147</v>
       </c>
       <c r="I38" s="11" t="n">
@@ -3023,7 +3006,7 @@
       <c r="G39" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="23" t="s">
         <v>154</v>
       </c>
       <c r="I39" s="11" t="n">
@@ -3057,13 +3040,13 @@
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
-      <c r="H40" s="26" t="s">
+      <c r="H40" s="23" t="s">
         <v>159</v>
       </c>
       <c r="I40" s="11" t="n">
         <v>37</v>
       </c>
-      <c r="J40" s="24"/>
+      <c r="J40" s="21"/>
       <c r="K40" s="8"/>
       <c r="L40" s="13" t="n">
         <v>-1</v>
@@ -3095,13 +3078,13 @@
       <c r="G41" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="H41" s="26" t="s">
+      <c r="H41" s="23" t="s">
         <v>166</v>
       </c>
       <c r="I41" s="11" t="n">
         <v>38</v>
       </c>
-      <c r="J41" s="24"/>
+      <c r="J41" s="21"/>
       <c r="K41" s="8"/>
       <c r="L41" s="18"/>
     </row>
@@ -3123,7 +3106,7 @@
         <v>58</v>
       </c>
       <c r="G42" s="11"/>
-      <c r="H42" s="26" t="s">
+      <c r="H42" s="23" t="s">
         <v>170</v>
       </c>
       <c r="I42" s="11" t="n">
@@ -3153,18 +3136,18 @@
       <c r="G43" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="H43" s="27" t="s">
+      <c r="H43" s="24" t="s">
         <v>176</v>
       </c>
       <c r="I43" s="11" t="n">
         <v>40</v>
       </c>
-      <c r="J43" s="24"/>
+      <c r="J43" s="21"/>
       <c r="K43" s="8"/>
-      <c r="L43" s="28" t="s">
+      <c r="L43" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M43" s="29" t="s">
+      <c r="M43" s="9" t="s">
         <v>177</v>
       </c>
       <c r="N43" s="10" t="s">
@@ -3189,15 +3172,15 @@
         <v>58</v>
       </c>
       <c r="G44" s="11"/>
-      <c r="H44" s="27" t="s">
+      <c r="H44" s="24" t="s">
         <v>181</v>
       </c>
       <c r="I44" s="11" t="n">
         <v>41</v>
       </c>
-      <c r="J44" s="24"/>
+      <c r="J44" s="21"/>
       <c r="K44" s="8"/>
-      <c r="L44" s="21" t="n">
+      <c r="L44" s="16" t="n">
         <v>86</v>
       </c>
       <c r="M44" s="12" t="s">
@@ -3225,15 +3208,15 @@
         <v>174</v>
       </c>
       <c r="G45" s="11"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="24" t="s">
         <v>185</v>
       </c>
       <c r="I45" s="11" t="n">
         <v>42</v>
       </c>
-      <c r="J45" s="24"/>
+      <c r="J45" s="21"/>
       <c r="K45" s="8"/>
-      <c r="L45" s="21" t="n">
+      <c r="L45" s="16" t="n">
         <v>87</v>
       </c>
       <c r="M45" s="12" t="s">
@@ -3259,15 +3242,15 @@
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
-      <c r="H46" s="27" t="s">
+      <c r="H46" s="24" t="s">
         <v>190</v>
       </c>
       <c r="I46" s="11" t="n">
         <v>43</v>
       </c>
-      <c r="J46" s="24"/>
+      <c r="J46" s="21"/>
       <c r="K46" s="8"/>
-      <c r="L46" s="21" t="n">
+      <c r="L46" s="16" t="n">
         <v>88</v>
       </c>
       <c r="M46" s="12" t="s">
@@ -3293,15 +3276,15 @@
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
-      <c r="H47" s="27" t="s">
+      <c r="H47" s="24" t="s">
         <v>195</v>
       </c>
       <c r="I47" s="11" t="n">
         <v>44</v>
       </c>
-      <c r="J47" s="24"/>
+      <c r="J47" s="21"/>
       <c r="K47" s="8"/>
-      <c r="L47" s="21" t="n">
+      <c r="L47" s="16" t="n">
         <v>89</v>
       </c>
       <c r="M47" s="12" t="s">
@@ -3339,7 +3322,7 @@
       <c r="I48" s="11" t="n">
         <v>45</v>
       </c>
-      <c r="J48" s="24"/>
+      <c r="J48" s="21"/>
       <c r="K48" s="8"/>
       <c r="L48" s="18"/>
     </row>
@@ -3371,7 +3354,7 @@
       <c r="I49" s="11" t="n">
         <v>46</v>
       </c>
-      <c r="J49" s="24"/>
+      <c r="J49" s="21"/>
       <c r="K49" s="8"/>
       <c r="L49" s="18"/>
     </row>
@@ -3403,14 +3386,14 @@
       <c r="I50" s="11" t="n">
         <v>47</v>
       </c>
-      <c r="J50" s="24" t="n">
+      <c r="J50" s="21" t="n">
         <v>9</v>
       </c>
       <c r="K50" s="8"/>
-      <c r="L50" s="28" t="s">
+      <c r="L50" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M50" s="29" t="s">
+      <c r="M50" s="9" t="s">
         <v>212</v>
       </c>
       <c r="N50" s="10" t="s">
@@ -3445,11 +3428,11 @@
       <c r="I51" s="11" t="n">
         <v>48</v>
       </c>
-      <c r="J51" s="24" t="n">
+      <c r="J51" s="21" t="n">
         <v>8</v>
       </c>
       <c r="K51" s="8"/>
-      <c r="L51" s="21" t="n">
+      <c r="L51" s="16" t="n">
         <v>75</v>
       </c>
       <c r="M51" s="12" t="s">
@@ -3477,11 +3460,11 @@
       <c r="I52" s="11" t="n">
         <v>49</v>
       </c>
-      <c r="J52" s="24" t="n">
+      <c r="J52" s="21" t="n">
         <v>7</v>
       </c>
       <c r="K52" s="8"/>
-      <c r="L52" s="21" t="n">
+      <c r="L52" s="16" t="n">
         <v>76</v>
       </c>
       <c r="M52" s="12" t="s">
@@ -3517,11 +3500,11 @@
       <c r="I53" s="11" t="n">
         <v>50</v>
       </c>
-      <c r="J53" s="24" t="n">
+      <c r="J53" s="21" t="n">
         <v>6</v>
       </c>
       <c r="K53" s="8"/>
-      <c r="L53" s="21" t="n">
+      <c r="L53" s="16" t="n">
         <v>77</v>
       </c>
       <c r="M53" s="12" t="s">
@@ -3555,11 +3538,11 @@
       <c r="I54" s="11" t="n">
         <v>51</v>
       </c>
-      <c r="J54" s="24" t="n">
+      <c r="J54" s="21" t="n">
         <v>5</v>
       </c>
       <c r="K54" s="8"/>
-      <c r="L54" s="21" t="n">
+      <c r="L54" s="16" t="n">
         <v>78</v>
       </c>
       <c r="M54" s="12" t="s">
@@ -3593,7 +3576,7 @@
       <c r="I55" s="11" t="n">
         <v>52</v>
       </c>
-      <c r="J55" s="24" t="n">
+      <c r="J55" s="21" t="n">
         <v>4</v>
       </c>
       <c r="K55" s="8"/>
@@ -3625,7 +3608,7 @@
       <c r="I56" s="11" t="n">
         <v>53</v>
       </c>
-      <c r="J56" s="24" t="n">
+      <c r="J56" s="21" t="n">
         <v>3</v>
       </c>
       <c r="K56" s="8"/>
@@ -3651,18 +3634,18 @@
       <c r="G57" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H57" s="30" t="s">
+      <c r="H57" s="25" t="s">
         <v>238</v>
       </c>
       <c r="I57" s="11" t="n">
         <v>54</v>
       </c>
-      <c r="J57" s="24"/>
+      <c r="J57" s="21"/>
       <c r="K57" s="8"/>
-      <c r="L57" s="28" t="s">
+      <c r="L57" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M57" s="29" t="s">
+      <c r="M57" s="9" t="s">
         <v>239</v>
       </c>
       <c r="N57" s="10" t="s">
@@ -3689,15 +3672,15 @@
       <c r="G58" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="H58" s="30" t="s">
+      <c r="H58" s="25" t="s">
         <v>244</v>
       </c>
       <c r="I58" s="11" t="n">
         <v>55</v>
       </c>
-      <c r="J58" s="24"/>
+      <c r="J58" s="21"/>
       <c r="K58" s="8"/>
-      <c r="L58" s="21" t="n">
+      <c r="L58" s="16" t="n">
         <v>90</v>
       </c>
       <c r="M58" s="12" t="s">
@@ -3727,15 +3710,15 @@
       <c r="G59" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H59" s="30" t="s">
+      <c r="H59" s="25" t="s">
         <v>251</v>
       </c>
       <c r="I59" s="11" t="n">
         <v>56</v>
       </c>
-      <c r="J59" s="24"/>
+      <c r="J59" s="21"/>
       <c r="K59" s="8"/>
-      <c r="L59" s="21" t="n">
+      <c r="L59" s="16" t="n">
         <v>91</v>
       </c>
       <c r="M59" s="12" t="s">
@@ -3763,15 +3746,15 @@
         <v>58</v>
       </c>
       <c r="G60" s="11"/>
-      <c r="H60" s="30" t="s">
+      <c r="H60" s="25" t="s">
         <v>257</v>
       </c>
       <c r="I60" s="11" t="n">
         <v>57</v>
       </c>
-      <c r="J60" s="24"/>
+      <c r="J60" s="21"/>
       <c r="K60" s="8"/>
-      <c r="L60" s="21" t="n">
+      <c r="L60" s="16" t="n">
         <v>92</v>
       </c>
       <c r="M60" s="12" t="s">
@@ -3797,15 +3780,15 @@
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
       <c r="G61" s="11"/>
-      <c r="H61" s="30" t="s">
+      <c r="H61" s="25" t="s">
         <v>262</v>
       </c>
       <c r="I61" s="11" t="n">
         <v>58</v>
       </c>
-      <c r="J61" s="24"/>
+      <c r="J61" s="21"/>
       <c r="K61" s="8"/>
-      <c r="L61" s="21" t="n">
+      <c r="L61" s="16" t="n">
         <v>93</v>
       </c>
       <c r="M61" s="12" t="s">
@@ -3835,15 +3818,15 @@
       <c r="G62" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="H62" s="31" t="s">
+      <c r="H62" s="26" t="s">
         <v>268</v>
       </c>
       <c r="I62" s="11" t="n">
         <v>59</v>
       </c>
-      <c r="J62" s="24"/>
+      <c r="J62" s="21"/>
       <c r="K62" s="8"/>
-      <c r="L62" s="21" t="n">
+      <c r="L62" s="16" t="n">
         <v>94</v>
       </c>
       <c r="M62" s="12" t="s">
@@ -3873,15 +3856,15 @@
       <c r="G63" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H63" s="31" t="s">
+      <c r="H63" s="26" t="s">
         <v>274</v>
       </c>
       <c r="I63" s="11" t="n">
         <v>60</v>
       </c>
-      <c r="J63" s="24"/>
+      <c r="J63" s="21"/>
       <c r="K63" s="8"/>
-      <c r="L63" s="21" t="n">
+      <c r="L63" s="16" t="n">
         <v>95</v>
       </c>
       <c r="M63" s="12" t="s">
@@ -3913,7 +3896,7 @@
       </c>
       <c r="J64" s="7"/>
       <c r="K64" s="8"/>
-      <c r="L64" s="21" t="n">
+      <c r="L64" s="16" t="n">
         <v>96</v>
       </c>
       <c r="M64" s="12" t="s">
@@ -3945,7 +3928,7 @@
       </c>
       <c r="J65" s="7"/>
       <c r="K65" s="8"/>
-      <c r="L65" s="21" t="n">
+      <c r="L65" s="16" t="n">
         <v>97</v>
       </c>
       <c r="M65" s="12" t="s">
@@ -3977,13 +3960,13 @@
       <c r="G66" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H66" s="31" t="s">
+      <c r="H66" s="26" t="s">
         <v>285</v>
       </c>
       <c r="I66" s="11" t="n">
         <v>63</v>
       </c>
-      <c r="J66" s="24"/>
+      <c r="J66" s="21"/>
       <c r="K66" s="8"/>
       <c r="L66" s="18"/>
     </row>
@@ -4009,13 +3992,13 @@
       <c r="G67" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="H67" s="31" t="s">
+      <c r="H67" s="26" t="s">
         <v>292</v>
       </c>
       <c r="I67" s="11" t="n">
         <v>64</v>
       </c>
-      <c r="J67" s="24"/>
+      <c r="J67" s="21"/>
       <c r="K67" s="8"/>
       <c r="L67" s="18"/>
     </row>
@@ -4041,20 +4024,20 @@
       <c r="G68" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H68" s="21" t="s">
+      <c r="H68" s="16" t="s">
         <v>294</v>
       </c>
       <c r="I68" s="11" t="n">
         <v>65</v>
       </c>
-      <c r="J68" s="24" t="n">
+      <c r="J68" s="21" t="n">
         <v>7</v>
       </c>
       <c r="K68" s="8"/>
-      <c r="L68" s="28" t="s">
+      <c r="L68" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M68" s="29" t="s">
+      <c r="M68" s="9" t="s">
         <v>295</v>
       </c>
       <c r="N68" s="10" t="s">
@@ -4083,17 +4066,17 @@
       <c r="G69" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H69" s="21" t="s">
+      <c r="H69" s="16" t="s">
         <v>294</v>
       </c>
       <c r="I69" s="11" t="n">
         <v>66</v>
       </c>
-      <c r="J69" s="24" t="n">
+      <c r="J69" s="21" t="n">
         <v>6</v>
       </c>
       <c r="K69" s="8"/>
-      <c r="L69" s="21" t="n">
+      <c r="L69" s="16" t="n">
         <v>83</v>
       </c>
       <c r="M69" s="12" t="s">
@@ -4125,17 +4108,17 @@
       <c r="G70" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H70" s="21" t="s">
+      <c r="H70" s="16" t="s">
         <v>294</v>
       </c>
       <c r="I70" s="11" t="n">
         <v>67</v>
       </c>
-      <c r="J70" s="24" t="n">
+      <c r="J70" s="21" t="n">
         <v>5</v>
       </c>
       <c r="K70" s="8"/>
-      <c r="L70" s="21" t="n">
+      <c r="L70" s="16" t="n">
         <v>84</v>
       </c>
       <c r="M70" s="12" t="s">
@@ -4167,17 +4150,17 @@
       <c r="G71" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H71" s="21" t="s">
+      <c r="H71" s="16" t="s">
         <v>294</v>
       </c>
       <c r="I71" s="11" t="n">
         <v>68</v>
       </c>
-      <c r="J71" s="24" t="n">
+      <c r="J71" s="21" t="n">
         <v>4</v>
       </c>
       <c r="K71" s="8"/>
-      <c r="L71" s="21" t="n">
+      <c r="L71" s="16" t="n">
         <v>95</v>
       </c>
       <c r="M71" s="12" t="s">
@@ -4209,17 +4192,17 @@
       <c r="G72" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H72" s="21" t="s">
+      <c r="H72" s="16" t="s">
         <v>294</v>
       </c>
       <c r="I72" s="11" t="n">
         <v>69</v>
       </c>
-      <c r="J72" s="24" t="n">
+      <c r="J72" s="21" t="n">
         <v>3</v>
       </c>
       <c r="K72" s="8"/>
-      <c r="L72" s="32"/>
+      <c r="L72" s="27"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="11" t="n">
@@ -4239,15 +4222,15 @@
         <v>58</v>
       </c>
       <c r="G73" s="11"/>
-      <c r="H73" s="31" t="s">
+      <c r="H73" s="26" t="s">
         <v>309</v>
       </c>
       <c r="I73" s="11" t="n">
         <v>70</v>
       </c>
-      <c r="J73" s="24"/>
-      <c r="K73" s="32"/>
-      <c r="L73" s="32"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="27"/>
+      <c r="L73" s="27"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="11" t="n">
@@ -4269,15 +4252,15 @@
       <c r="G74" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="H74" s="31" t="s">
+      <c r="H74" s="26" t="s">
         <v>314</v>
       </c>
       <c r="I74" s="11" t="n">
         <v>71</v>
       </c>
-      <c r="J74" s="24"/>
-      <c r="K74" s="32"/>
-      <c r="L74" s="32"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="27"/>
+      <c r="L74" s="27"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="11" t="n">
@@ -4299,14 +4282,14 @@
       <c r="G75" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="H75" s="33" t="s">
+      <c r="H75" s="28" t="s">
         <v>320</v>
       </c>
       <c r="I75" s="11" t="n">
         <v>72</v>
       </c>
-      <c r="J75" s="24"/>
-      <c r="K75" s="32"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="27"/>
       <c r="L75" s="18"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4329,14 +4312,14 @@
       <c r="G76" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="H76" s="31" t="s">
+      <c r="H76" s="26" t="s">
         <v>325</v>
       </c>
       <c r="I76" s="11" t="n">
         <v>73</v>
       </c>
-      <c r="J76" s="24"/>
-      <c r="K76" s="32"/>
+      <c r="J76" s="21"/>
+      <c r="K76" s="27"/>
       <c r="L76" s="18"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4359,14 +4342,14 @@
       <c r="G77" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="H77" s="31" t="s">
+      <c r="H77" s="26" t="s">
         <v>331</v>
       </c>
       <c r="I77" s="11" t="n">
         <v>74</v>
       </c>
-      <c r="J77" s="24"/>
-      <c r="K77" s="32"/>
+      <c r="J77" s="21"/>
+      <c r="K77" s="27"/>
       <c r="L77" s="18"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4389,14 +4372,14 @@
       <c r="G78" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="H78" s="31" t="s">
+      <c r="H78" s="26" t="s">
         <v>336</v>
       </c>
       <c r="I78" s="11" t="n">
         <v>75</v>
       </c>
-      <c r="J78" s="24"/>
-      <c r="K78" s="32"/>
+      <c r="J78" s="21"/>
+      <c r="K78" s="27"/>
       <c r="L78" s="18"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4419,14 +4402,14 @@
       <c r="G79" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="H79" s="25" t="s">
+      <c r="H79" s="22" t="s">
         <v>342</v>
       </c>
       <c r="I79" s="11" t="n">
         <v>76</v>
       </c>
-      <c r="J79" s="24"/>
-      <c r="K79" s="32"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="27"/>
       <c r="L79" s="18"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4449,13 +4432,13 @@
       <c r="G80" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="H80" s="21" t="s">
+      <c r="H80" s="16" t="s">
         <v>347</v>
       </c>
       <c r="I80" s="11" t="n">
         <v>77</v>
       </c>
-      <c r="J80" s="24"/>
+      <c r="J80" s="21"/>
       <c r="K80" s="18"/>
       <c r="L80" s="18"/>
     </row>
@@ -4475,13 +4458,13 @@
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
       <c r="G81" s="11"/>
-      <c r="H81" s="21" t="s">
+      <c r="H81" s="16" t="s">
         <v>351</v>
       </c>
       <c r="I81" s="11" t="n">
         <v>78</v>
       </c>
-      <c r="J81" s="24"/>
+      <c r="J81" s="21"/>
       <c r="K81" s="18"/>
       <c r="L81" s="18"/>
     </row>
@@ -4568,61 +4551,61 @@
       <c r="L84" s="18"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="19" t="n">
+      <c r="A85" s="11" t="n">
         <v>82</v>
       </c>
-      <c r="B85" s="19" t="s">
+      <c r="B85" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="D85" s="19" t="s">
+      <c r="D85" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="E85" s="19"/>
-      <c r="F85" s="20" t="s">
+      <c r="E85" s="11"/>
+      <c r="F85" s="17" t="s">
         <v>356</v>
       </c>
-      <c r="G85" s="19" t="s">
+      <c r="G85" s="11" t="s">
         <v>88</v>
       </c>
       <c r="H85" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="I85" s="19" t="n">
+      <c r="I85" s="11" t="n">
         <v>82</v>
       </c>
-      <c r="J85" s="24" t="n">
+      <c r="J85" s="21" t="n">
         <v>1</v>
       </c>
       <c r="K85" s="8"/>
       <c r="L85" s="18"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="19" t="n">
+      <c r="A86" s="11" t="n">
         <v>83</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="B86" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="C86" s="19" t="s">
+      <c r="C86" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="D86" s="19" t="s">
+      <c r="D86" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="E86" s="19"/>
-      <c r="F86" s="20" t="s">
+      <c r="E86" s="11"/>
+      <c r="F86" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="G86" s="19" t="s">
+      <c r="G86" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="H86" s="34" t="s">
+      <c r="H86" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="I86" s="19" t="n">
+      <c r="I86" s="11" t="n">
         <v>83</v>
       </c>
       <c r="J86" s="7"/>
@@ -4630,29 +4613,29 @@
       <c r="L86" s="18"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="19" t="n">
+      <c r="A87" s="11" t="n">
         <v>84</v>
       </c>
-      <c r="B87" s="19" t="s">
+      <c r="B87" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="C87" s="19" t="s">
+      <c r="C87" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="D87" s="19" t="s">
+      <c r="D87" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="E87" s="19"/>
-      <c r="F87" s="20" t="s">
+      <c r="E87" s="11"/>
+      <c r="F87" s="17" t="s">
         <v>364</v>
       </c>
-      <c r="G87" s="19" t="s">
+      <c r="G87" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="H87" s="35" t="s">
+      <c r="H87" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="I87" s="19" t="n">
+      <c r="I87" s="11" t="n">
         <v>84</v>
       </c>
       <c r="J87" s="7"/>
@@ -4675,7 +4658,7 @@
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
-      <c r="H88" s="34" t="s">
+      <c r="H88" s="29" t="s">
         <v>369</v>
       </c>
       <c r="I88" s="11" t="n">
@@ -4701,13 +4684,13 @@
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
-      <c r="H89" s="36" t="s">
+      <c r="H89" s="31" t="s">
         <v>373</v>
       </c>
       <c r="I89" s="11" t="n">
         <v>86</v>
       </c>
-      <c r="J89" s="24"/>
+      <c r="J89" s="21"/>
       <c r="K89" s="8"/>
       <c r="L89" s="18"/>
     </row>
@@ -4727,13 +4710,13 @@
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
-      <c r="H90" s="36" t="s">
+      <c r="H90" s="31" t="s">
         <v>377</v>
       </c>
       <c r="I90" s="11" t="n">
         <v>87</v>
       </c>
-      <c r="J90" s="24"/>
+      <c r="J90" s="21"/>
       <c r="K90" s="18"/>
       <c r="L90" s="18"/>
     </row>
@@ -4753,14 +4736,14 @@
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
       <c r="G91" s="11"/>
-      <c r="H91" s="36" t="s">
+      <c r="H91" s="31" t="s">
         <v>381</v>
       </c>
       <c r="I91" s="11" t="n">
         <v>88</v>
       </c>
-      <c r="J91" s="24"/>
-      <c r="K91" s="32"/>
+      <c r="J91" s="21"/>
+      <c r="K91" s="27"/>
       <c r="L91" s="18"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4783,13 +4766,13 @@
       <c r="G92" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="H92" s="36" t="s">
+      <c r="H92" s="31" t="s">
         <v>387</v>
       </c>
       <c r="I92" s="11" t="n">
         <v>89</v>
       </c>
-      <c r="J92" s="24"/>
+      <c r="J92" s="21"/>
       <c r="K92" s="8"/>
       <c r="L92" s="18"/>
     </row>
@@ -4813,7 +4796,7 @@
       <c r="G93" s="11" t="s">
         <v>392</v>
       </c>
-      <c r="H93" s="37" t="s">
+      <c r="H93" s="32" t="s">
         <v>393</v>
       </c>
       <c r="I93" s="11" t="n">
@@ -4843,7 +4826,7 @@
       <c r="G94" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="H94" s="37" t="s">
+      <c r="H94" s="32" t="s">
         <v>399</v>
       </c>
       <c r="I94" s="11" t="n">
@@ -4869,7 +4852,7 @@
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
       <c r="G95" s="11"/>
-      <c r="H95" s="37" t="s">
+      <c r="H95" s="32" t="s">
         <v>313</v>
       </c>
       <c r="I95" s="11" t="n">
@@ -4895,7 +4878,7 @@
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
       <c r="G96" s="11"/>
-      <c r="H96" s="37" t="s">
+      <c r="H96" s="32" t="s">
         <v>324</v>
       </c>
       <c r="I96" s="11" t="n">
@@ -4921,7 +4904,7 @@
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
       <c r="G97" s="11"/>
-      <c r="H97" s="37" t="s">
+      <c r="H97" s="32" t="s">
         <v>335</v>
       </c>
       <c r="I97" s="11" t="n">
@@ -4951,7 +4934,7 @@
       <c r="G98" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="H98" s="37" t="s">
+      <c r="H98" s="32" t="s">
         <v>346</v>
       </c>
       <c r="I98" s="11" t="n">
@@ -4981,7 +4964,7 @@
       <c r="G99" s="11" t="s">
         <v>417</v>
       </c>
-      <c r="H99" s="37" t="s">
+      <c r="H99" s="32" t="s">
         <v>418</v>
       </c>
       <c r="I99" s="11" t="n">
@@ -5011,7 +4994,7 @@
       <c r="G100" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="H100" s="37" t="s">
+      <c r="H100" s="32" t="s">
         <v>66</v>
       </c>
       <c r="I100" s="11" t="n">
@@ -5090,6 +5073,11 @@
       <c r="J103" s="7"/>
       <c r="K103" s="8"/>
       <c r="L103" s="18"/>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="0" t="s">
+        <v>426</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5119,7 +5107,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5146,11 +5134,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>